<commit_message>
fix welcome page issue
</commit_message>
<xml_diff>
--- a/storage/app/xlsx/invoices.xlsx
+++ b/storage/app/xlsx/invoices.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denis\Projects\2hex\storage\app\xlsx\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27760" windowHeight="15640"/>
   </bookViews>
   <sheets>
     <sheet name="INVOICE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mgSyc4HwyJB06AciDaWNxuakqHQAQ=="/>
     </ext>
@@ -143,7 +141,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00"/>
   </numFmts>
@@ -439,7 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -667,24 +665,24 @@
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.75" customWidth="1"/>
-    <col min="2" max="2" width="4.125" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" customWidth="1"/>
     <col min="3" max="7" width="10.5" customWidth="1"/>
     <col min="8" max="9" width="12" customWidth="1"/>
     <col min="10" max="10" width="25" customWidth="1"/>
     <col min="11" max="11" width="15.5" customWidth="1"/>
-    <col min="12" max="12" width="13.125" customWidth="1"/>
-    <col min="13" max="13" width="11.625" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
     <col min="14" max="14" width="10.5" customWidth="1"/>
-    <col min="15" max="15" width="4.125" customWidth="1"/>
+    <col min="15" max="15" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" ht="15.75" customHeight="1">
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" ht="15.75" customHeight="1">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -700,7 +698,7 @@
       <c r="N2" s="3"/>
       <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="2:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" ht="36" customHeight="1">
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -716,7 +714,7 @@
       <c r="N3" s="6"/>
       <c r="O3" s="7"/>
     </row>
-    <row r="4" spans="2:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:15" ht="39.75" customHeight="1">
       <c r="B4" s="5"/>
       <c r="C4" s="8" t="s">
         <v>0</v>
@@ -734,7 +732,7 @@
       <c r="N4" s="6"/>
       <c r="O4" s="7"/>
     </row>
-    <row r="5" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" ht="15.75" customHeight="1">
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -750,7 +748,7 @@
       <c r="N5" s="6"/>
       <c r="O5" s="7"/>
     </row>
-    <row r="6" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" ht="15.75" customHeight="1">
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -766,7 +764,7 @@
       <c r="N6" s="6"/>
       <c r="O6" s="7"/>
     </row>
-    <row r="7" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" ht="15.75" customHeight="1">
       <c r="B7" s="5"/>
       <c r="C7" s="9" t="s">
         <v>1</v>
@@ -788,7 +786,7 @@
       </c>
       <c r="O7" s="7"/>
     </row>
-    <row r="8" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" ht="15.75" customHeight="1">
       <c r="B8" s="5"/>
       <c r="C8" s="9" t="s">
         <v>4</v>
@@ -810,7 +808,7 @@
       </c>
       <c r="O8" s="7"/>
     </row>
-    <row r="9" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" ht="15.75" customHeight="1">
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -830,7 +828,7 @@
       </c>
       <c r="O9" s="7"/>
     </row>
-    <row r="10" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" ht="15.75" customHeight="1">
       <c r="B10" s="5"/>
       <c r="C10" s="6" t="s">
         <v>9</v>
@@ -852,7 +850,7 @@
       </c>
       <c r="O10" s="7"/>
     </row>
-    <row r="11" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" ht="15.75" customHeight="1">
       <c r="B11" s="5"/>
       <c r="C11" s="9" t="s">
         <v>12</v>
@@ -876,7 +874,7 @@
       </c>
       <c r="O11" s="7"/>
     </row>
-    <row r="12" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" ht="15.75" customHeight="1">
       <c r="B12" s="5"/>
       <c r="C12" s="9" t="s">
         <v>16</v>
@@ -898,7 +896,7 @@
       <c r="N12" s="6"/>
       <c r="O12" s="7"/>
     </row>
-    <row r="13" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" ht="15.75" customHeight="1">
       <c r="B13" s="5"/>
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
@@ -914,7 +912,7 @@
       <c r="N13" s="35"/>
       <c r="O13" s="7"/>
     </row>
-    <row r="14" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" ht="15.75" customHeight="1">
       <c r="B14" s="5"/>
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
@@ -930,7 +928,7 @@
       <c r="N14" s="35"/>
       <c r="O14" s="7"/>
     </row>
-    <row r="15" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" ht="15.75" customHeight="1">
       <c r="B15" s="5"/>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
@@ -946,7 +944,7 @@
       <c r="N15" s="35"/>
       <c r="O15" s="7"/>
     </row>
-    <row r="16" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" ht="15.75" customHeight="1">
       <c r="B16" s="5"/>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
@@ -962,7 +960,7 @@
       <c r="N16" s="35"/>
       <c r="O16" s="7"/>
     </row>
-    <row r="17" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" ht="15.75" customHeight="1">
       <c r="B17" s="5"/>
       <c r="C17" s="33"/>
       <c r="D17" s="33"/>
@@ -978,7 +976,7 @@
       <c r="N17" s="35"/>
       <c r="O17" s="7"/>
     </row>
-    <row r="18" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" ht="15.75" customHeight="1">
       <c r="B18" s="5"/>
       <c r="C18" s="16" t="s">
         <v>19</v>
@@ -996,7 +994,7 @@
       <c r="N18" s="6"/>
       <c r="O18" s="7"/>
     </row>
-    <row r="19" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" ht="15.75" customHeight="1">
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -1012,7 +1010,7 @@
       <c r="N19" s="6"/>
       <c r="O19" s="7"/>
     </row>
-    <row r="20" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" ht="15.75" customHeight="1">
       <c r="B20" s="5"/>
       <c r="C20" s="6" t="s">
         <v>10</v>
@@ -1030,7 +1028,7 @@
       <c r="N20" s="6"/>
       <c r="O20" s="7"/>
     </row>
-    <row r="21" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" ht="15.75" customHeight="1">
       <c r="B21" s="5"/>
       <c r="C21" s="6" t="s">
         <v>20</v>
@@ -1048,7 +1046,7 @@
       <c r="N21" s="6"/>
       <c r="O21" s="7"/>
     </row>
-    <row r="22" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" ht="15.75" customHeight="1">
       <c r="B22" s="5"/>
       <c r="C22" s="6" t="s">
         <v>21</v>
@@ -1066,7 +1064,7 @@
       <c r="N22" s="6"/>
       <c r="O22" s="7"/>
     </row>
-    <row r="23" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" ht="15.75" customHeight="1">
       <c r="B23" s="5"/>
       <c r="C23" s="6" t="s">
         <v>7</v>
@@ -1084,7 +1082,7 @@
       <c r="N23" s="6"/>
       <c r="O23" s="7"/>
     </row>
-    <row r="24" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" ht="15.75" customHeight="1">
       <c r="B24" s="5"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1100,7 +1098,7 @@
       <c r="N24" s="6"/>
       <c r="O24" s="7"/>
     </row>
-    <row r="25" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" ht="15.75" customHeight="1">
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -1116,7 +1114,7 @@
       <c r="N25" s="6"/>
       <c r="O25" s="7"/>
     </row>
-    <row r="26" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" ht="15.75" customHeight="1">
       <c r="B26" s="5"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -1132,7 +1130,7 @@
       <c r="N26" s="6"/>
       <c r="O26" s="7"/>
     </row>
-    <row r="27" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:15" ht="15.75" customHeight="1">
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -1148,7 +1146,7 @@
       <c r="N27" s="6"/>
       <c r="O27" s="7"/>
     </row>
-    <row r="28" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" ht="15.75" customHeight="1">
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
@@ -1164,7 +1162,7 @@
       <c r="N28" s="6"/>
       <c r="O28" s="7"/>
     </row>
-    <row r="29" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15" ht="15.75" customHeight="1">
       <c r="B29" s="5"/>
       <c r="C29" s="21" t="s">
         <v>22</v>
@@ -1182,7 +1180,7 @@
       <c r="N29" s="22"/>
       <c r="O29" s="7"/>
     </row>
-    <row r="30" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15" ht="15.75" customHeight="1">
       <c r="B30" s="5"/>
       <c r="C30" s="25"/>
       <c r="D30" s="6"/>
@@ -1198,7 +1196,7 @@
       <c r="N30" s="6"/>
       <c r="O30" s="7"/>
     </row>
-    <row r="31" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" ht="15.75" customHeight="1">
       <c r="B31" s="5"/>
       <c r="C31" s="9" t="s">
         <v>23</v>
@@ -1226,7 +1224,7 @@
       <c r="N31" s="27"/>
       <c r="O31" s="7"/>
     </row>
-    <row r="32" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" ht="15.75" customHeight="1">
       <c r="B32" s="5"/>
       <c r="C32" s="9" t="s">
         <v>28</v>
@@ -1254,7 +1252,7 @@
       <c r="N32" s="27"/>
       <c r="O32" s="7"/>
     </row>
-    <row r="33" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" ht="15.75" customHeight="1">
       <c r="B33" s="5"/>
       <c r="C33" s="6" t="s">
         <v>34</v>
@@ -1274,7 +1272,7 @@
       <c r="N33" s="6"/>
       <c r="O33" s="7"/>
     </row>
-    <row r="34" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15" ht="15.75" customHeight="1">
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
@@ -1290,7 +1288,7 @@
       <c r="N34" s="6"/>
       <c r="O34" s="7"/>
     </row>
-    <row r="35" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" ht="15.75" customHeight="1">
       <c r="B35" s="5"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
@@ -1306,7 +1304,7 @@
       <c r="N35" s="6"/>
       <c r="O35" s="7"/>
     </row>
-    <row r="36" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15" ht="15.75" customHeight="1">
       <c r="B36" s="5"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
@@ -1322,7 +1320,7 @@
       <c r="N36" s="6"/>
       <c r="O36" s="7"/>
     </row>
-    <row r="37" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15" ht="15.75" customHeight="1">
       <c r="B37" s="5"/>
       <c r="C37" s="28" t="s">
         <v>36</v>
@@ -1340,7 +1338,7 @@
       <c r="N37" s="28"/>
       <c r="O37" s="7"/>
     </row>
-    <row r="38" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:15" ht="15.75" customHeight="1">
       <c r="B38" s="5"/>
       <c r="C38" s="29" t="s">
         <v>37</v>
@@ -1358,7 +1356,7 @@
       <c r="N38" s="29"/>
       <c r="O38" s="7"/>
     </row>
-    <row r="39" spans="2:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:15" ht="18.75" customHeight="1">
       <c r="B39" s="30"/>
       <c r="C39" s="31"/>
       <c r="D39" s="31"/>
@@ -1374,1361 +1372,1361 @@
       <c r="N39" s="31"/>
       <c r="O39" s="32"/>
     </row>
-    <row r="40" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15" ht="15.75" customHeight="1">
       <c r="O40" s="1"/>
     </row>
-    <row r="41" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:15" ht="15.75" customHeight="1">
       <c r="O41" s="1"/>
     </row>
-    <row r="42" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15" ht="15.75" customHeight="1">
       <c r="O42" s="1"/>
     </row>
-    <row r="43" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:15" ht="15.75" customHeight="1">
       <c r="O43" s="1"/>
     </row>
-    <row r="44" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:15" ht="15.75" customHeight="1">
       <c r="O44" s="1"/>
     </row>
-    <row r="45" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:15" ht="15.75" customHeight="1">
       <c r="O45" s="1"/>
     </row>
-    <row r="46" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:15" ht="15.75" customHeight="1">
       <c r="O46" s="1"/>
     </row>
-    <row r="47" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:15" ht="15.75" customHeight="1">
       <c r="O47" s="1"/>
     </row>
-    <row r="48" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15" ht="15.75" customHeight="1">
       <c r="O48" s="1"/>
     </row>
-    <row r="49" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="15:15" ht="15.75" customHeight="1">
       <c r="O49" s="1"/>
     </row>
-    <row r="50" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="15:15" ht="15.75" customHeight="1">
       <c r="O50" s="1"/>
     </row>
-    <row r="51" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="15:15" ht="15.75" customHeight="1">
       <c r="O51" s="1"/>
     </row>
-    <row r="52" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="15:15" ht="15.75" customHeight="1">
       <c r="O52" s="1"/>
     </row>
-    <row r="53" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="15:15" ht="15.75" customHeight="1">
       <c r="O53" s="1"/>
     </row>
-    <row r="54" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="15:15" ht="15.75" customHeight="1">
       <c r="O54" s="1"/>
     </row>
-    <row r="55" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="15:15" ht="15.75" customHeight="1">
       <c r="O55" s="1"/>
     </row>
-    <row r="56" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="15:15" ht="15.75" customHeight="1">
       <c r="O56" s="1"/>
     </row>
-    <row r="57" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="15:15" ht="15.75" customHeight="1">
       <c r="O57" s="1"/>
     </row>
-    <row r="58" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="15:15" ht="15.75" customHeight="1">
       <c r="O58" s="1"/>
     </row>
-    <row r="59" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="15:15" ht="15.75" customHeight="1">
       <c r="O59" s="1"/>
     </row>
-    <row r="60" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="15:15" ht="15.75" customHeight="1">
       <c r="O60" s="1"/>
     </row>
-    <row r="61" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="15:15" ht="15.75" customHeight="1">
       <c r="O61" s="1"/>
     </row>
-    <row r="62" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="15:15" ht="15.75" customHeight="1">
       <c r="O62" s="1"/>
     </row>
-    <row r="63" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="15:15" ht="15.75" customHeight="1">
       <c r="O63" s="1"/>
     </row>
-    <row r="64" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="15:15" ht="15.75" customHeight="1">
       <c r="O64" s="1"/>
     </row>
-    <row r="65" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="15:15" ht="15.75" customHeight="1">
       <c r="O65" s="1"/>
     </row>
-    <row r="66" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="15:15" ht="15.75" customHeight="1">
       <c r="O66" s="1"/>
     </row>
-    <row r="67" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="15:15" ht="15.75" customHeight="1">
       <c r="O67" s="1"/>
     </row>
-    <row r="68" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="15:15" ht="15.75" customHeight="1">
       <c r="O68" s="1"/>
     </row>
-    <row r="69" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="15:15" ht="15.75" customHeight="1">
       <c r="O69" s="1"/>
     </row>
-    <row r="70" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="15:15" ht="15.75" customHeight="1">
       <c r="O70" s="1"/>
     </row>
-    <row r="71" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="15:15" ht="15.75" customHeight="1">
       <c r="O71" s="1"/>
     </row>
-    <row r="72" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="15:15" ht="15.75" customHeight="1">
       <c r="O72" s="1"/>
     </row>
-    <row r="73" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="15:15" ht="15.75" customHeight="1">
       <c r="O73" s="1"/>
     </row>
-    <row r="74" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="15:15" ht="15.75" customHeight="1">
       <c r="O74" s="1"/>
     </row>
-    <row r="75" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="15:15" ht="15.75" customHeight="1">
       <c r="O75" s="1"/>
     </row>
-    <row r="76" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="15:15" ht="15.75" customHeight="1">
       <c r="O76" s="1"/>
     </row>
-    <row r="77" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="15:15" ht="15.75" customHeight="1">
       <c r="O77" s="1"/>
     </row>
-    <row r="78" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="15:15" ht="15.75" customHeight="1">
       <c r="O78" s="1"/>
     </row>
-    <row r="79" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="15:15" ht="15.75" customHeight="1">
       <c r="O79" s="1"/>
     </row>
-    <row r="80" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="15:15" ht="15.75" customHeight="1">
       <c r="O80" s="1"/>
     </row>
-    <row r="81" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="15:15" ht="15.75" customHeight="1">
       <c r="O81" s="1"/>
     </row>
-    <row r="82" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="15:15" ht="15.75" customHeight="1">
       <c r="O82" s="1"/>
     </row>
-    <row r="83" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="15:15" ht="15.75" customHeight="1">
       <c r="O83" s="1"/>
     </row>
-    <row r="84" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="15:15" ht="15.75" customHeight="1">
       <c r="O84" s="1"/>
     </row>
-    <row r="85" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="15:15" ht="15.75" customHeight="1">
       <c r="O85" s="1"/>
     </row>
-    <row r="86" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="15:15" ht="15.75" customHeight="1">
       <c r="O86" s="1"/>
     </row>
-    <row r="87" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="15:15" ht="15.75" customHeight="1">
       <c r="O87" s="1"/>
     </row>
-    <row r="88" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="15:15" ht="15.75" customHeight="1">
       <c r="O88" s="1"/>
     </row>
-    <row r="89" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="15:15" ht="15.75" customHeight="1">
       <c r="O89" s="1"/>
     </row>
-    <row r="90" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="15:15" ht="15.75" customHeight="1">
       <c r="O90" s="1"/>
     </row>
-    <row r="91" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="15:15" ht="15.75" customHeight="1">
       <c r="O91" s="1"/>
     </row>
-    <row r="92" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="15:15" ht="15.75" customHeight="1">
       <c r="O92" s="1"/>
     </row>
-    <row r="93" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="15:15" ht="15.75" customHeight="1">
       <c r="O93" s="1"/>
     </row>
-    <row r="94" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="15:15" ht="15.75" customHeight="1">
       <c r="O94" s="1"/>
     </row>
-    <row r="95" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="15:15" ht="15.75" customHeight="1">
       <c r="O95" s="1"/>
     </row>
-    <row r="96" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="15:15" ht="15.75" customHeight="1">
       <c r="O96" s="1"/>
     </row>
-    <row r="97" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="15:15" ht="15.75" customHeight="1">
       <c r="O97" s="1"/>
     </row>
-    <row r="98" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="15:15" ht="15.75" customHeight="1">
       <c r="O98" s="1"/>
     </row>
-    <row r="99" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="15:15" ht="15.75" customHeight="1">
       <c r="O99" s="1"/>
     </row>
-    <row r="100" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="15:15" ht="15.75" customHeight="1">
       <c r="O100" s="1"/>
     </row>
-    <row r="101" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="15:15" ht="15.75" customHeight="1">
       <c r="O101" s="1"/>
     </row>
-    <row r="102" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="15:15" ht="15.75" customHeight="1">
       <c r="O102" s="1"/>
     </row>
-    <row r="103" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="15:15" ht="15.75" customHeight="1">
       <c r="O103" s="1"/>
     </row>
-    <row r="104" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="15:15" ht="15.75" customHeight="1">
       <c r="O104" s="1"/>
     </row>
-    <row r="105" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="15:15" ht="15.75" customHeight="1">
       <c r="O105" s="1"/>
     </row>
-    <row r="106" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="15:15" ht="15.75" customHeight="1">
       <c r="O106" s="1"/>
     </row>
-    <row r="107" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="15:15" ht="15.75" customHeight="1">
       <c r="O107" s="1"/>
     </row>
-    <row r="108" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="15:15" ht="15.75" customHeight="1">
       <c r="O108" s="1"/>
     </row>
-    <row r="109" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="15:15" ht="15.75" customHeight="1">
       <c r="O109" s="1"/>
     </row>
-    <row r="110" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="15:15" ht="15.75" customHeight="1">
       <c r="O110" s="1"/>
     </row>
-    <row r="111" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="15:15" ht="15.75" customHeight="1">
       <c r="O111" s="1"/>
     </row>
-    <row r="112" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="15:15" ht="15.75" customHeight="1">
       <c r="O112" s="1"/>
     </row>
-    <row r="113" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="15:15" ht="15.75" customHeight="1">
       <c r="O113" s="1"/>
     </row>
-    <row r="114" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="15:15" ht="15.75" customHeight="1">
       <c r="O114" s="1"/>
     </row>
-    <row r="115" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="15:15" ht="15.75" customHeight="1">
       <c r="O115" s="1"/>
     </row>
-    <row r="116" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="15:15" ht="15.75" customHeight="1">
       <c r="O116" s="1"/>
     </row>
-    <row r="117" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="15:15" ht="15.75" customHeight="1">
       <c r="O117" s="1"/>
     </row>
-    <row r="118" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="15:15" ht="15.75" customHeight="1">
       <c r="O118" s="1"/>
     </row>
-    <row r="119" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="15:15" ht="15.75" customHeight="1">
       <c r="O119" s="1"/>
     </row>
-    <row r="120" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="15:15" ht="15.75" customHeight="1">
       <c r="O120" s="1"/>
     </row>
-    <row r="121" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="15:15" ht="15.75" customHeight="1">
       <c r="O121" s="1"/>
     </row>
-    <row r="122" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="15:15" ht="15.75" customHeight="1">
       <c r="O122" s="1"/>
     </row>
-    <row r="123" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="15:15" ht="15.75" customHeight="1">
       <c r="O123" s="1"/>
     </row>
-    <row r="124" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="15:15" ht="15.75" customHeight="1">
       <c r="O124" s="1"/>
     </row>
-    <row r="125" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="15:15" ht="15.75" customHeight="1">
       <c r="O125" s="1"/>
     </row>
-    <row r="126" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="15:15" ht="15.75" customHeight="1">
       <c r="O126" s="1"/>
     </row>
-    <row r="127" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="15:15" ht="15.75" customHeight="1">
       <c r="O127" s="1"/>
     </row>
-    <row r="128" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="15:15" ht="15.75" customHeight="1">
       <c r="O128" s="1"/>
     </row>
-    <row r="129" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="15:15" ht="15.75" customHeight="1">
       <c r="O129" s="1"/>
     </row>
-    <row r="130" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="15:15" ht="15.75" customHeight="1">
       <c r="O130" s="1"/>
     </row>
-    <row r="131" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="15:15" ht="15.75" customHeight="1">
       <c r="O131" s="1"/>
     </row>
-    <row r="132" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="15:15" ht="15.75" customHeight="1">
       <c r="O132" s="1"/>
     </row>
-    <row r="133" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="15:15" ht="15.75" customHeight="1">
       <c r="O133" s="1"/>
     </row>
-    <row r="134" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="15:15" ht="15.75" customHeight="1">
       <c r="O134" s="1"/>
     </row>
-    <row r="135" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="15:15" ht="15.75" customHeight="1">
       <c r="O135" s="1"/>
     </row>
-    <row r="136" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="15:15" ht="15.75" customHeight="1">
       <c r="O136" s="1"/>
     </row>
-    <row r="137" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="15:15" ht="15.75" customHeight="1">
       <c r="O137" s="1"/>
     </row>
-    <row r="138" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="15:15" ht="15.75" customHeight="1">
       <c r="O138" s="1"/>
     </row>
-    <row r="139" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="15:15" ht="15.75" customHeight="1">
       <c r="O139" s="1"/>
     </row>
-    <row r="140" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="15:15" ht="15.75" customHeight="1">
       <c r="O140" s="1"/>
     </row>
-    <row r="141" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="15:15" ht="15.75" customHeight="1">
       <c r="O141" s="1"/>
     </row>
-    <row r="142" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="15:15" ht="15.75" customHeight="1">
       <c r="O142" s="1"/>
     </row>
-    <row r="143" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="15:15" ht="15.75" customHeight="1">
       <c r="O143" s="1"/>
     </row>
-    <row r="144" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="15:15" ht="15.75" customHeight="1">
       <c r="O144" s="1"/>
     </row>
-    <row r="145" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="15:15" ht="15.75" customHeight="1">
       <c r="O145" s="1"/>
     </row>
-    <row r="146" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="15:15" ht="15.75" customHeight="1">
       <c r="O146" s="1"/>
     </row>
-    <row r="147" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="15:15" ht="15.75" customHeight="1">
       <c r="O147" s="1"/>
     </row>
-    <row r="148" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="15:15" ht="15.75" customHeight="1">
       <c r="O148" s="1"/>
     </row>
-    <row r="149" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="15:15" ht="15.75" customHeight="1">
       <c r="O149" s="1"/>
     </row>
-    <row r="150" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="15:15" ht="15.75" customHeight="1">
       <c r="O150" s="1"/>
     </row>
-    <row r="151" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="15:15" ht="15.75" customHeight="1">
       <c r="O151" s="1"/>
     </row>
-    <row r="152" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="15:15" ht="15.75" customHeight="1">
       <c r="O152" s="1"/>
     </row>
-    <row r="153" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="15:15" ht="15.75" customHeight="1">
       <c r="O153" s="1"/>
     </row>
-    <row r="154" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="15:15" ht="15.75" customHeight="1">
       <c r="O154" s="1"/>
     </row>
-    <row r="155" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="15:15" ht="15.75" customHeight="1">
       <c r="O155" s="1"/>
     </row>
-    <row r="156" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="15:15" ht="15.75" customHeight="1">
       <c r="O156" s="1"/>
     </row>
-    <row r="157" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="15:15" ht="15.75" customHeight="1">
       <c r="O157" s="1"/>
     </row>
-    <row r="158" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="15:15" ht="15.75" customHeight="1">
       <c r="O158" s="1"/>
     </row>
-    <row r="159" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="15:15" ht="15.75" customHeight="1">
       <c r="O159" s="1"/>
     </row>
-    <row r="160" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="15:15" ht="15.75" customHeight="1">
       <c r="O160" s="1"/>
     </row>
-    <row r="161" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="15:15" ht="15.75" customHeight="1">
       <c r="O161" s="1"/>
     </row>
-    <row r="162" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="15:15" ht="15.75" customHeight="1">
       <c r="O162" s="1"/>
     </row>
-    <row r="163" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="15:15" ht="15.75" customHeight="1">
       <c r="O163" s="1"/>
     </row>
-    <row r="164" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="15:15" ht="15.75" customHeight="1">
       <c r="O164" s="1"/>
     </row>
-    <row r="165" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="15:15" ht="15.75" customHeight="1">
       <c r="O165" s="1"/>
     </row>
-    <row r="166" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="15:15" ht="15.75" customHeight="1">
       <c r="O166" s="1"/>
     </row>
-    <row r="167" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="15:15" ht="15.75" customHeight="1">
       <c r="O167" s="1"/>
     </row>
-    <row r="168" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="15:15" ht="15.75" customHeight="1">
       <c r="O168" s="1"/>
     </row>
-    <row r="169" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="15:15" ht="15.75" customHeight="1">
       <c r="O169" s="1"/>
     </row>
-    <row r="170" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="15:15" ht="15.75" customHeight="1">
       <c r="O170" s="1"/>
     </row>
-    <row r="171" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="15:15" ht="15.75" customHeight="1">
       <c r="O171" s="1"/>
     </row>
-    <row r="172" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="15:15" ht="15.75" customHeight="1">
       <c r="O172" s="1"/>
     </row>
-    <row r="173" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="15:15" ht="15.75" customHeight="1">
       <c r="O173" s="1"/>
     </row>
-    <row r="174" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="15:15" ht="15.75" customHeight="1">
       <c r="O174" s="1"/>
     </row>
-    <row r="175" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="15:15" ht="15.75" customHeight="1">
       <c r="O175" s="1"/>
     </row>
-    <row r="176" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="15:15" ht="15.75" customHeight="1">
       <c r="O176" s="1"/>
     </row>
-    <row r="177" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="15:15" ht="15.75" customHeight="1">
       <c r="O177" s="1"/>
     </row>
-    <row r="178" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="15:15" ht="15.75" customHeight="1">
       <c r="O178" s="1"/>
     </row>
-    <row r="179" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="15:15" ht="15.75" customHeight="1">
       <c r="O179" s="1"/>
     </row>
-    <row r="180" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="15:15" ht="15.75" customHeight="1">
       <c r="O180" s="1"/>
     </row>
-    <row r="181" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="15:15" ht="15.75" customHeight="1">
       <c r="O181" s="1"/>
     </row>
-    <row r="182" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="15:15" ht="15.75" customHeight="1">
       <c r="O182" s="1"/>
     </row>
-    <row r="183" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="15:15" ht="15.75" customHeight="1">
       <c r="O183" s="1"/>
     </row>
-    <row r="184" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="15:15" ht="15.75" customHeight="1">
       <c r="O184" s="1"/>
     </row>
-    <row r="185" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="15:15" ht="15.75" customHeight="1">
       <c r="O185" s="1"/>
     </row>
-    <row r="186" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="15:15" ht="15.75" customHeight="1">
       <c r="O186" s="1"/>
     </row>
-    <row r="187" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="15:15" ht="15.75" customHeight="1">
       <c r="O187" s="1"/>
     </row>
-    <row r="188" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="15:15" ht="15.75" customHeight="1">
       <c r="O188" s="1"/>
     </row>
-    <row r="189" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="15:15" ht="15.75" customHeight="1">
       <c r="O189" s="1"/>
     </row>
-    <row r="190" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="15:15" ht="15.75" customHeight="1">
       <c r="O190" s="1"/>
     </row>
-    <row r="191" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="15:15" ht="15.75" customHeight="1">
       <c r="O191" s="1"/>
     </row>
-    <row r="192" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="15:15" ht="15.75" customHeight="1">
       <c r="O192" s="1"/>
     </row>
-    <row r="193" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="15:15" ht="15.75" customHeight="1">
       <c r="O193" s="1"/>
     </row>
-    <row r="194" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="15:15" ht="15.75" customHeight="1">
       <c r="O194" s="1"/>
     </row>
-    <row r="195" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="15:15" ht="15.75" customHeight="1">
       <c r="O195" s="1"/>
     </row>
-    <row r="196" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="15:15" ht="15.75" customHeight="1">
       <c r="O196" s="1"/>
     </row>
-    <row r="197" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="15:15" ht="15.75" customHeight="1">
       <c r="O197" s="1"/>
     </row>
-    <row r="198" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="15:15" ht="15.75" customHeight="1">
       <c r="O198" s="1"/>
     </row>
-    <row r="199" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="15:15" ht="15.75" customHeight="1">
       <c r="O199" s="1"/>
     </row>
-    <row r="200" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="15:15" ht="15.75" customHeight="1">
       <c r="O200" s="1"/>
     </row>
-    <row r="201" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="15:15" ht="15.75" customHeight="1">
       <c r="O201" s="1"/>
     </row>
-    <row r="202" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="15:15" ht="15.75" customHeight="1">
       <c r="O202" s="1"/>
     </row>
-    <row r="203" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="15:15" ht="15.75" customHeight="1">
       <c r="O203" s="1"/>
     </row>
-    <row r="204" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="15:15" ht="15.75" customHeight="1">
       <c r="O204" s="1"/>
     </row>
-    <row r="205" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="15:15" ht="15.75" customHeight="1">
       <c r="O205" s="1"/>
     </row>
-    <row r="206" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="15:15" ht="15.75" customHeight="1">
       <c r="O206" s="1"/>
     </row>
-    <row r="207" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="15:15" ht="15.75" customHeight="1">
       <c r="O207" s="1"/>
     </row>
-    <row r="208" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="15:15" ht="15.75" customHeight="1">
       <c r="O208" s="1"/>
     </row>
-    <row r="209" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="15:15" ht="15.75" customHeight="1">
       <c r="O209" s="1"/>
     </row>
-    <row r="210" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="15:15" ht="15.75" customHeight="1">
       <c r="O210" s="1"/>
     </row>
-    <row r="211" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="15:15" ht="15.75" customHeight="1">
       <c r="O211" s="1"/>
     </row>
-    <row r="212" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="15:15" ht="15.75" customHeight="1">
       <c r="O212" s="1"/>
     </row>
-    <row r="213" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="15:15" ht="15.75" customHeight="1">
       <c r="O213" s="1"/>
     </row>
-    <row r="214" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="15:15" ht="15.75" customHeight="1">
       <c r="O214" s="1"/>
     </row>
-    <row r="215" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="15:15" ht="15.75" customHeight="1">
       <c r="O215" s="1"/>
     </row>
-    <row r="216" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="15:15" ht="15.75" customHeight="1">
       <c r="O216" s="1"/>
     </row>
-    <row r="217" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="15:15" ht="15.75" customHeight="1">
       <c r="O217" s="1"/>
     </row>
-    <row r="218" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="15:15" ht="15.75" customHeight="1">
       <c r="O218" s="1"/>
     </row>
-    <row r="219" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="15:15" ht="15.75" customHeight="1">
       <c r="O219" s="1"/>
     </row>
-    <row r="220" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="15:15" ht="15.75" customHeight="1">
       <c r="O220" s="1"/>
     </row>
-    <row r="221" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="15:15" ht="15.75" customHeight="1">
       <c r="O221" s="1"/>
     </row>
-    <row r="222" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="15:15" ht="15.75" customHeight="1">
       <c r="O222" s="1"/>
     </row>
-    <row r="223" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="15:15" ht="15.75" customHeight="1">
       <c r="O223" s="1"/>
     </row>
-    <row r="224" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="15:15" ht="15.75" customHeight="1">
       <c r="O224" s="1"/>
     </row>
-    <row r="225" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="15:15" ht="15.75" customHeight="1">
       <c r="O225" s="1"/>
     </row>
-    <row r="226" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="15:15" ht="15.75" customHeight="1">
       <c r="O226" s="1"/>
     </row>
-    <row r="227" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="15:15" ht="15.75" customHeight="1">
       <c r="O227" s="1"/>
     </row>
-    <row r="228" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="15:15" ht="15.75" customHeight="1">
       <c r="O228" s="1"/>
     </row>
-    <row r="229" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="15:15" ht="15.75" customHeight="1">
       <c r="O229" s="1"/>
     </row>
-    <row r="230" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="15:15" ht="15.75" customHeight="1">
       <c r="O230" s="1"/>
     </row>
-    <row r="231" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="15:15" ht="15.75" customHeight="1">
       <c r="O231" s="1"/>
     </row>
-    <row r="232" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="15:15" ht="15.75" customHeight="1">
       <c r="O232" s="1"/>
     </row>
-    <row r="233" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="15:15" ht="15.75" customHeight="1">
       <c r="O233" s="1"/>
     </row>
-    <row r="234" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="15:15" ht="15.75" customHeight="1">
       <c r="O234" s="1"/>
     </row>
-    <row r="235" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="15:15" ht="15.75" customHeight="1">
       <c r="O235" s="1"/>
     </row>
-    <row r="236" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="15:15" ht="15.75" customHeight="1">
       <c r="O236" s="1"/>
     </row>
-    <row r="237" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="15:15" ht="15.75" customHeight="1">
       <c r="O237" s="1"/>
     </row>
-    <row r="238" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="15:15" ht="15.75" customHeight="1">
       <c r="O238" s="1"/>
     </row>
-    <row r="239" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" spans="15:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" spans="15:15" ht="15.75" customHeight="1"/>
+    <row r="240" spans="15:15" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G22:M27"/>
@@ -2742,6 +2740,10 @@
     <hyperlink ref="E11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>